<commit_message>
add EnemyGroupManager, add Effect,Texture
</commit_message>
<xml_diff>
--- a/AxisShootingDoc/memo.xlsx
+++ b/AxisShootingDoc/memo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>・プレイヤー</t>
     <phoneticPr fontId="1"/>
@@ -65,10 +65,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>・エフェクト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・リソース差し替え</t>
     <rPh sb="5" eb="6">
       <t>サ</t>
@@ -84,6 +80,71 @@
   </si>
   <si>
     <t>・シーンマネージャー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>残機制御</t>
+    <rPh sb="0" eb="2">
+      <t>ザンキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>セイギョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プレイヤービーム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・爆発エフェクト</t>
+    <rPh sb="1" eb="3">
+      <t>バクハツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エネミーグループマネージャー作成</t>
+    <rPh sb="14" eb="16">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>→</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エネミーが入ってる親を生成
+子のエネミーがすべて死亡
+orステージ外に消えたら　次のグループ生成</t>
+    <rPh sb="5" eb="6">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>オヤ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シボウ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ガイ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>セイセイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -139,10 +200,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -423,16 +487,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B14"/>
+  <dimension ref="B3:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="31.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.4">
@@ -456,7 +521,7 @@
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -466,33 +531,54 @@
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
-        <v>8</v>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>